<commit_message>
Text editors functions study v2
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Text editors functions study.xlsx
+++ b/TypeCobol/Documentation/Studies/Text editors functions study.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Text editors" sheetId="1" r:id="rId1"/>
+    <sheet name="TypeCobol interfaces" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="228">
   <si>
     <t>Visual Studio</t>
   </si>
@@ -81,9 +82,6 @@
   </si>
   <si>
     <t>http://confluence.jetbrains.com/display/IDEADEV/Developing+Custom+Language+Plugins+for+IntelliJ+IDEA</t>
-  </si>
-  <si>
-    <t>https://github.com/JetBrains/intellij-community/tree/7c8377934c3c433b75ef79c7bc28dddb8cc4b21c/platform/core-api/src/com/intellij/openapi/editor</t>
   </si>
   <si>
     <t>com.intellij.openapi.editor.Document</t>
@@ -292,11 +290,6 @@
   <si>
     <t>Tracking.TrackPositionForwardInTime
 Traverse a linked list of ITextVersion from orginal snapshot to target snapshot, study each ITextChange in ITextVersion.Changes and compute if it modified the indexes of the bounds of the orginal span</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LineSpan IStgringRebuilder.GetLineFromLineNumber(int lineNumber)
-Each IStringRebuilder node holds a LineBreakCount property
-Recursive traversal of the binary tree enables to find the right nodes wich contribute to one line </t>
   </si>
   <si>
     <t>ITextSnapshot.LineCount
@@ -700,12 +693,247 @@
   <si>
     <t>org.eclipse.jface.text.FindReplaceDocumentAdapter</t>
   </si>
+  <si>
+    <t>void LoadChars(IEnumerable&lt;char&gt; textSource)</t>
+  </si>
+  <si>
+    <t>char CharAt(int offset);</t>
+  </si>
+  <si>
+    <t>string TextSegment(int startOffset, int endOffset)</t>
+  </si>
+  <si>
+    <t>int Length { get; }</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Used by</t>
+  </si>
+  <si>
+    <t>CompilationDocument(string libraryName, string textName, ...)
+ObserverTextDocument.OnNext(CobolFileChangedEvent value)
+TextDocument(string fileName, IEnumerable&lt;char&gt; textSource ...)</t>
+  </si>
+  <si>
+    <t>TextDocumentCharStream.La(int i)</t>
+  </si>
+  <si>
+    <t>TextDocumentCharStream.GetText(Interval interval)</t>
+  </si>
+  <si>
+    <t>TextDocumentCharStream(ITextDocument document, int currentOffset)</t>
+  </si>
+  <si>
+    <t>TokensDocument.OnNext(TextChangedEvent textChangedEvent)</t>
+  </si>
+  <si>
+    <t>TokensDocument.OnNext(TextChangedEvent textChangedEvent)
+TokensDocument.PropagateChangeAfterLine(int updatedLineIndex,…)</t>
+  </si>
+  <si>
+    <t>ITextLine GetLineByIndex(int lineIndex)</t>
+  </si>
+  <si>
+    <t>ITextLine GetLineByOffset(int offset, out int indexOfCharInLine)</t>
+  </si>
+  <si>
+    <t>int LineCount { get; }</t>
+  </si>
+  <si>
+    <t>IObservable&lt;TextChangedEvent&gt; TextChangedEventsSource { get; }</t>
+  </si>
+  <si>
+    <t>void StartSendingChangeEvents()</t>
+  </si>
+  <si>
+    <t>string FileName { get; }</t>
+  </si>
+  <si>
+    <t>TextChangedEvent</t>
+  </si>
+  <si>
+    <t>CompilationDocument.SetupDocumentProcessingPipeline(...)</t>
+  </si>
+  <si>
+    <t>CompilationDocument.StartDocumentProcessing()
+CompilationDocument.StartContinuousFileProcessing()</t>
+  </si>
+  <si>
+    <t>TextDocumentCharStream(ITextDocument document, int currentOffset)
+TokensDocumentTokenSource.SourceName
+CopyTokensLinesIterator.DocumentPath
+ProcessedTokensDocument.OnNext(...)
+TokensDocument.SourceTokens</t>
+  </si>
+  <si>
+    <t>IList&lt;TextChange&gt; TextChanges { get; private set; }</t>
+  </si>
+  <si>
+    <t>TextChange</t>
+  </si>
+  <si>
+    <t>ColumnsLayout ColumnsLayout { get; }</t>
+  </si>
+  <si>
+    <t>TextChangeType Type { get; private set; }</t>
+  </si>
+  <si>
+    <t>int LineIndex { get; private set; }</t>
+  </si>
+  <si>
+    <t>ITextLine NewLine { get; private set; }</t>
+  </si>
+  <si>
+    <t>ITextLine</t>
+  </si>
+  <si>
+    <t>int LineIndex { get; }</t>
+  </si>
+  <si>
+    <t>int StartOffset { get; }</t>
+  </si>
+  <si>
+    <t>string Text { get; }</t>
+  </si>
+  <si>
+    <t>string TextSegment(int startIndex, int endIndexInclusive)</t>
+  </si>
+  <si>
+    <t>Token.LineIndex
+Token.Line
+TextDocument.TextSegment(...)
+TextDocument/AvalonEditTextDocument.SendSocumentChangeEvent()
+AvalonEditTextDocument.RebuildDocument()</t>
+  </si>
+  <si>
+    <t>CopyTokensLinesIterator.Offset
+TokensLinesIterator.Offset
+TextDocument.GetLineByOffset(…)</t>
+  </si>
+  <si>
+    <t>TextDocument.TextSegment(int startOffset, int endOffset)
+TextDocument.LoadChars(IEnumerable&lt;char&gt; textSource)</t>
+  </si>
+  <si>
+    <t>Scanner.ScanTokensLine(TokensLine tokensLine, …)
+TextDocument.CharAt(int offset)
+TextDocument.TextSegment(int startOffset, int endOffset)
+TextLineMap.MapVariableLengthLineWithReferenceFormat()
+TextLineMap.MapVariableLengthLineWithFreeFormat()
+TextLine.TextSegment(int startIndex, int endIndexInclusive)
+TextLine.Length</t>
+  </si>
+  <si>
+    <t>Token.SourceText
+TextDocument.TextSegment(int startOffset, int endOffset)
+TextLineMap.SequenceNumberText / IndicatorChar / SourceText / CommentText</t>
+  </si>
+  <si>
+    <t>Implementation : AvalonEditTextDocument</t>
+  </si>
+  <si>
+    <t>ITextDocument =&gt; returns values from the "live" buffer</t>
+  </si>
+  <si>
+    <t>ITextLine =&gt; immutable copy  of the line properties (string and integer duplication) in the methods ITextDocument.GetLineByXxx()</t>
+  </si>
+  <si>
+    <t>TextChangedEvents =&gt; based on the "live" (new) line numbers &amp; the new text line is always a copy of the original buffer</t>
+  </si>
+  <si>
+    <t>ICSharpCode.AvalonEdit.Document.DocumentLine</t>
+  </si>
+  <si>
+    <t>DebugVerifyAccess() / VerifyAccess()</t>
+  </si>
+  <si>
+    <t>SetOwnerThread(Thread newOwner)</t>
+  </si>
+  <si>
+    <t>TextDocument can be accessed only from the thread that owns it.</t>
+  </si>
+  <si>
+    <t>protect document change against corruption by other changes inside the event handlers</t>
+  </si>
+  <si>
+    <t>ITextSource CreateSnapshot()</t>
+  </si>
+  <si>
+    <t>DocumentLineTree</t>
+  </si>
+  <si>
+    <t>IsInBeginUpdate / Replace / EndUpdate : IsInUpdate</t>
+  </si>
+  <si>
+    <t>is updated by LineManager from the TextDocument.ReplaceMethod
+thus updated by the owner thread
+=&gt; DocumentLine properties can only be accessed from the owner thread</t>
+  </si>
+  <si>
+    <t>node in the DocumentLineTree
+totalLength and delimiter length stored once in DLT.InsertLineAfter()
+IsDeleted stored by DocumentLineTree.RemoveNode
+LineNumber and Offset dynamically computed on the DocumentLineTree</t>
+  </si>
+  <si>
+    <t>Creates an immutable snapshot of this text source. 
+Unlike all other methods in this interface, this method is thread-safe. 
+=&gt; but creates only a snapshot of the text, NOT of the document lines &amp; text anchors</t>
+  </si>
+  <si>
+    <t>Thread-safety: a TextSegmentCollection that is connected to a &lt;see cref="TextDocument"/&gt; may only be used on that document's owner thread.</t>
+  </si>
+  <si>
+    <t>Can only read the TextAnchor offset property from the owner thread</t>
+  </si>
+  <si>
+    <t>Because TextAnchorTree is updated in the Replace method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LineSpan IStringRebuilder.GetLineFromLineNumber(int lineNumber)
+Each IStringRebuilder node holds a LineBreakCount property
+Recursive traversal of the binary tree enables to find the right nodes wich contribute to one line </t>
+  </si>
+  <si>
+    <t>Conclusion : Visual Studio text document is the only one which is truly multi-thread</t>
+  </si>
+  <si>
+    <t>Then Intellij &amp; SharpDevelop enable text only snapshots</t>
+  </si>
+  <si>
+    <t>Then Eclipse &amp; Netbeans provide no multi-thread option</t>
+  </si>
+  <si>
+    <t>https://github.com/JetBrains/intellij-community/tree/7c8377934c3c433b75ef79c7bc28dddb8cc4b21c/platform/core-impl/src/com/intellij/openapi/editor/impl</t>
+  </si>
+  <si>
+    <t>JAVA RECONCILER</t>
+  </si>
+  <si>
+    <t>org.eclipse.jdt.internal.ui.text.java.JavaReconcilingStrategy.reconcile()
+org.eclipse.jdt.internal.core.CompilationUnit.reconcile()
+org.eclipse.jdt.internal.core.ReconcileWorkingCopyOperation.makeConsistent()
+org.eclipse.jdt.internal.core.CompilationUnit.openBuffer()
+org.eclipse.jdt.internal.core.BufferManager</t>
+  </si>
+  <si>
+    <t>=&gt; the Java reconciler :
+- ignores the dirty region received as parameter
+- does not use the IDocument implementation of the editor
+- uses its own org.eclipse.jdt.internal.core.Buffer in the background thread (a simple gap buffer)
+- this buffer is updated ... to do ... ???</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,6 +959,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -769,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -786,6 +1021,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1068,13 +1318,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1353,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -1111,7 +1361,7 @@
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1119,22 +1369,22 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -1143,22 +1393,22 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H5" s="5"/>
     </row>
@@ -1167,22 +1417,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -1191,19 +1441,19 @@
         <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1211,13 +1461,13 @@
         <v>17</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1225,25 +1475,25 @@
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -1251,259 +1501,259 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>220</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1513,19 +1763,19 @@
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1535,93 +1785,93 @@
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1630,14 +1880,14 @@
     </row>
     <row r="30" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1646,14 +1896,14 @@
     </row>
     <row r="31" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1662,7 +1912,7 @@
     </row>
     <row r="32" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1673,48 +1923,63 @@
     </row>
     <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D39" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D40" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D42" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="D45" s="13" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1760,4 +2025,307 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId38"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B39" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="B48" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B49" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B55" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove all references to the source ITextDocument in the compilation pipeline : in most editors, the document in the IDE can only be accessed from the UI thread
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Text editors functions study.xlsx
+++ b/TypeCobol/Documentation/Studies/Text editors functions study.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Text editors" sheetId="1" r:id="rId1"/>
     <sheet name="TypeCobol interfaces" sheetId="2" r:id="rId2"/>
+    <sheet name="Steps data" sheetId="4" r:id="rId3"/>
+    <sheet name="Threads operations" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="287">
   <si>
     <t>Visual Studio</t>
   </si>
@@ -928,12 +930,217 @@
 - uses its own org.eclipse.jdt.internal.core.Buffer in the background thread (a simple gap buffer)
 - this buffer is updated ... to do ... ???</t>
   </si>
+  <si>
+    <t>TokensDocument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>public IObservable&lt;TokensChangedEvent&gt; TokensChangedEventsSource</t>
+  </si>
+  <si>
+    <t>Encoding EncodingForHexadecimalAlphanumericLiterals { get; private set; }</t>
+  </si>
+  <si>
+    <t>ITextDocument TextDocument { get; private set; }</t>
+  </si>
+  <si>
+    <t>TypeCobolOptions CompilerOptions { get; private set; }</t>
+  </si>
+  <si>
+    <t>IReadOnlyList&lt;TokensLine&gt; TokensLines { get { return tokensLines; } }</t>
+  </si>
+  <si>
+    <t>IEnumerable&lt;Token&gt; SourceTokens</t>
+  </si>
+  <si>
+    <t>SyntaxDocument.OnNext</t>
+  </si>
+  <si>
+    <t>new TokensDocumentTokenSource(ITextDocument)</t>
+  </si>
+  <si>
+    <t>ProcessedTokensDocument.GetTokensIterator</t>
+  </si>
+  <si>
+    <t>ProcessedTokensDocument.OnNext</t>
+  </si>
+  <si>
+    <t>new TokensLinesIterator(ITextDocument.FileName)</t>
+  </si>
+  <si>
+    <t>TokensDocument.SourceTokens</t>
+  </si>
+  <si>
+    <t>TokensDocument.OnNext</t>
+  </si>
+  <si>
+    <t>Scanner.ScanTextLine(ITextDocument.ColumnsLayout)</t>
+  </si>
+  <si>
+    <t>Scanner.ScanFirstLine(Encoding)</t>
+  </si>
+  <si>
+    <t>Scanner.ScanTextLine(CompilerOptions)</t>
+  </si>
+  <si>
+    <t>CompilationDocument.Diagnostics</t>
+  </si>
+  <si>
+    <t>foreach(TokensLine line in TokensDocument.TokensLines)</t>
+  </si>
+  <si>
+    <t>new TokensLinesIterator(TokensDocument.TokensLines)</t>
+  </si>
+  <si>
+    <t>TokensDocument.GetDebugString</t>
+  </si>
+  <si>
+    <t>SyntaxHighlighter.ColorizeLine</t>
+  </si>
+  <si>
+    <t>TokensDocument.TokensLines[lineIndex]</t>
+  </si>
+  <si>
+    <t>TestTokenSource.Check_CobolTokenSource_WithStartToken</t>
+  </si>
+  <si>
+    <t>CompilationDocument.SetupDocumentProcessingPipeline</t>
+  </si>
+  <si>
+    <t>TokensChangedEventsSource.Subscribe(ProcessedTokensDocument)</t>
+  </si>
+  <si>
+    <t>new TypeCobolCompilerService</t>
+  </si>
+  <si>
+    <t>// Refresh the syntax coloring for rescanned lines
+TokensChangedEventsSource.Subscribe(textEditor)</t>
+  </si>
+  <si>
+    <t>return textDocument.FileName</t>
+  </si>
+  <si>
+    <t>new CopyTokensLinesIterator(ITextDocument.FileName)</t>
+  </si>
+  <si>
+    <t>TokensDocumentTokenSource</t>
+  </si>
+  <si>
+    <t>ITokenSource.InputStream</t>
+  </si>
+  <si>
+    <t>new TextDocumentCharStream(textDocument, currentOffset)</t>
+  </si>
+  <si>
+    <t>ITokenSource.SourceName</t>
+  </si>
+  <si>
+    <t>DefaultErrorStrategy.ConstructToken</t>
+  </si>
+  <si>
+    <t>ITokenFactory.Create(current.TokenSource.InputStream)</t>
+  </si>
+  <si>
+    <t>TestTokenSource.Check_CobolTokenSource</t>
+  </si>
+  <si>
+    <t>TokensDocumentTokenSource.NextToken</t>
+  </si>
+  <si>
+    <t>nextToken.SetAntlrSource(this.InputStream)</t>
+  </si>
+  <si>
+    <t>tokenSource.TokenFactory.Create(tokenSource.InputStream)</t>
+  </si>
+  <si>
+    <t>IToken.InputStream</t>
+  </si>
+  <si>
+    <t>IToken.TokenSource</t>
+  </si>
+  <si>
+    <t>CobolTokenFactory.Create</t>
+  </si>
+  <si>
+    <t>Called by</t>
+  </si>
+  <si>
+    <t>Implemented in</t>
+  </si>
+  <si>
+    <t>ITokenFactory.Create</t>
+  </si>
+  <si>
+    <t>CommonTokenFactory.Create</t>
+  </si>
+  <si>
+    <t>CommonToken t = new CommonToken(source, ...
+if (copyText &amp;&amp; source.Item2 != null)
+    t.Text = source.Item2.GetText(Interval.Of(start, stop));</t>
+  </si>
+  <si>
+    <t>token.SetAntlrSource(source)</t>
+  </si>
+  <si>
+    <t>ITokenFactory factory = tokenSource.TokenFactory;
+factory.Create(Tuple.Create(current.TokenSource.InputStream …</t>
+  </si>
+  <si>
+    <t>CommonToken.Text</t>
+  </si>
+  <si>
+    <t>return input.GetText(Interval.Of(start, stop))</t>
+  </si>
+  <si>
+    <t>DefaultErrorStrategy.GetMissingSymbol(Parser recognizer)</t>
+  </si>
+  <si>
+    <t>return factory.Create(Tuple.Create(tokenSource, current.TokenSource.InputStream), expectedTokenType, tokenText, TokenConstants.DefaultChannel, -1, -1, current.Line, current.Column);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IToken currentSymbol = recognizer.CurrentToken;
+tokenText = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>recognizer.Vocabulary.GetDisplayName</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(expectedTokenType);
+ConstructToken(((ITokenStream)recognizer.InputStream).TokenSource, expectedTokenType, tokenText, current)</t>
+    </r>
+  </si>
+  <si>
+    <t>ITokenStream tokens = ((ITokenStream)recognizer.InputStream);</t>
+  </si>
+  <si>
+    <t>string input = tokens.GetText(e.StartToken, e.OffendingToken);</t>
+  </si>
+  <si>
+    <t>DefaultErrorStrategy.ReportNoViableAlternative</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -970,8 +1177,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -990,6 +1205,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1004,7 +1231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1037,6 +1264,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1320,11 +1553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,7 +2264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
@@ -2328,4 +2561,347 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>249</v>
+      </c>
+      <c r="D15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>239</v>
+      </c>
+      <c r="D16" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D22" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>255</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>260</v>
+      </c>
+      <c r="D26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>262</v>
+      </c>
+      <c r="D27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>263</v>
+      </c>
+      <c r="D30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D32" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>275</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>271</v>
+      </c>
+      <c r="D45" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>281</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="19" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug in relative path for TypeCobol.Test project
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Text editors functions study.xlsx
+++ b/TypeCobol/Documentation/Studies/Text editors functions study.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="7125" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Text editors" sheetId="1" r:id="rId1"/>
     <sheet name="TypeCobol interfaces" sheetId="2" r:id="rId2"/>
-    <sheet name="Steps data" sheetId="4" r:id="rId3"/>
-    <sheet name="Threads operations" sheetId="3" r:id="rId4"/>
+    <sheet name="Steps data (old)" sheetId="4" r:id="rId3"/>
+    <sheet name="Line changes" sheetId="5" r:id="rId4"/>
+    <sheet name="TypeCobol Steps" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="361">
   <si>
     <t>Visual Studio</t>
   </si>
@@ -941,9 +942,6 @@
   </si>
   <si>
     <t>Encoding EncodingForHexadecimalAlphanumericLiterals { get; private set; }</t>
-  </si>
-  <si>
-    <t>ITextDocument TextDocument { get; private set; }</t>
   </si>
   <si>
     <t>TypeCobolOptions CompilerOptions { get; private set; }</t>
@@ -1135,12 +1133,242 @@
   <si>
     <t>DefaultErrorStrategy.ReportNoViableAlternative</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ILineTracker
+void BeforeRemoveLine(DocumentLine line)
+void SetLineLength(DocumentLine line, int newTotalLength)
+void LineInserted(DocumentLine insertionPos, DocumentLine newLine)
+void RebuildDocument()</t>
+  </si>
+  <si>
+    <t>WeakLineTracker wlt
+textDocument.LineTrackers.Add(wlt);</t>
+  </si>
+  <si>
+    <t>TextSourceInfo</t>
+  </si>
+  <si>
+    <t>TypeCobolOptions</t>
+  </si>
+  <si>
+    <t>IReadOnlyList&lt;TokensLine&gt;</t>
+  </si>
+  <si>
+    <t>IEnumerable&lt;Token&gt;</t>
+  </si>
+  <si>
+    <t>&gt; TextChangedEvent &gt;</t>
+  </si>
+  <si>
+    <t>IList&lt;TextChange&gt;</t>
+  </si>
+  <si>
+    <t>- TextChangeType</t>
+  </si>
+  <si>
+    <t>- LineIndex</t>
+  </si>
+  <si>
+    <t>- ITextLine NewLine</t>
+  </si>
+  <si>
+    <t>&gt; TokensChangedEvent &gt;</t>
+  </si>
+  <si>
+    <t>IList&lt;TokensChange&gt;</t>
+  </si>
+  <si>
+    <t>- TokensChangeType</t>
+  </si>
+  <si>
+    <t>- TokensLine NewLine</t>
+  </si>
+  <si>
+    <t>IReadOnlyList&lt;ProcessedTokensLine&gt;</t>
+  </si>
+  <si>
+    <t>ProcessedTokensDocument</t>
+  </si>
+  <si>
+    <t>ITokensLinesIterator</t>
+  </si>
+  <si>
+    <t>- TextLineMap</t>
+  </si>
+  <si>
+    <t>- IList&lt;Diagnostic&gt; ScannerDiagnostics</t>
+  </si>
+  <si>
+    <t>- MultilineScanState(s)</t>
+  </si>
+  <si>
+    <t>- TokensLine</t>
+  </si>
+  <si>
+    <t>- PreprocessorState</t>
+  </si>
+  <si>
+    <t>- IList&lt;Token&gt; TokensWithCompilerDirectives</t>
+  </si>
+  <si>
+    <t>- IList&lt;Token&gt; SourceTokens</t>
+  </si>
+  <si>
+    <t>- CompilerListingControlDirective</t>
+  </si>
+  <si>
+    <t>- ImportedDocuments</t>
+  </si>
+  <si>
+    <t>- ReplaceDirective</t>
+  </si>
+  <si>
+    <t>- IList&lt;Diagnostic&gt; PreprocessorDiagnostics</t>
+  </si>
+  <si>
+    <t>- IsContinuedFromPreviousLine</t>
+  </si>
+  <si>
+    <t>- UsedLastTokenOfPreviousLine</t>
+  </si>
+  <si>
+    <t>- CopyTokensLinesIterator</t>
+  </si>
+  <si>
+    <t>- ReplaceTokensLinesIterator</t>
+  </si>
+  <si>
+    <t>SyntaxDocument</t>
+  </si>
+  <si>
+    <t>IList&lt;CodeElement&gt;</t>
+  </si>
+  <si>
+    <t>IList&lt;Diagnostic&gt; Diagnostics</t>
+  </si>
+  <si>
+    <t>TextLine</t>
+  </si>
+  <si>
+    <t>TextLineMap</t>
+  </si>
+  <si>
+    <t>IList&lt;Token&gt; SourceTokens</t>
+  </si>
+  <si>
+    <t>IList&lt;Diagnostic&gt; ScannerDiagnostics</t>
+  </si>
+  <si>
+    <t>IList&lt;Token&gt; TokensWithCompilerDirectives</t>
+  </si>
+  <si>
+    <t>IList&lt;Diagnostic&gt; PreprocessorDiagnostics</t>
+  </si>
+  <si>
+    <t>IList&lt;CodeElement&gt; CodeElements</t>
+  </si>
+  <si>
+    <t>IList&lt;Diagnostic&gt; ProgramClassParserDiagnostics</t>
+  </si>
+  <si>
+    <t>IList&lt;Diagnostic&gt; CodeElementsParserDiagnostics</t>
+  </si>
+  <si>
+    <t>TextLinesSnapshot</t>
+  </si>
+  <si>
+    <t>TextLinesVersion</t>
+  </si>
+  <si>
+    <t>- TextLinesVersion</t>
+  </si>
+  <si>
+    <t>- IReadOnlyList&lt;TextLine&gt;</t>
+  </si>
+  <si>
+    <t>ITextDocument.CurrentSnapshot</t>
+  </si>
+  <si>
+    <t>&lt;= UI thread only</t>
+  </si>
+  <si>
+    <t>&lt;= Background thread</t>
+  </si>
+  <si>
+    <t>ITextDocument.TryGetPosition(TextLine, start, stop)</t>
+  </si>
+  <si>
+    <t>- CompareAge</t>
+  </si>
+  <si>
+    <t>- GetChangesTo</t>
+  </si>
+  <si>
+    <t>- TextSpanMarker</t>
+  </si>
+  <si>
+    <t>VersionedList&lt;TListElement,TElementChangeEvent&gt;</t>
+  </si>
+  <si>
+    <t>VersionedListSnapshot&lt;TListElement,TElementChangeEvent&gt;</t>
+  </si>
+  <si>
+    <t>VersionedListRenderer</t>
+  </si>
+  <si>
+    <t>- RenderNewListVersion(VersionedListSnapshot)</t>
+  </si>
+  <si>
+    <t>Events listener on syntax elements registered on UI thread</t>
+  </si>
+  <si>
+    <t>- LastVersionRendered</t>
+  </si>
+  <si>
+    <t>- RenderChanges(TElementChangeEvent - from LastVersionRendered, TextLinesChanges - from CurrentSnapshot + PositionsAdapter)</t>
+  </si>
+  <si>
+    <t>(using TextSpanMarker)</t>
+  </si>
+  <si>
+    <t>- ForgetPreviousHistory</t>
+  </si>
+  <si>
+    <t>-- UI thread</t>
+  </si>
+  <si>
+    <t>-- Background thread</t>
+  </si>
+  <si>
+    <t>&gt; send events listener signal on UI thread</t>
+  </si>
+  <si>
+    <t>&gt; listeners list only accessed on UI thread</t>
+  </si>
+  <si>
+    <t>Change event optimization : New document / Document rebuilt</t>
+  </si>
+  <si>
+    <t>TextLinesToCodeElementsMap</t>
+  </si>
+  <si>
+    <t>CodeElementsToSyntaxListsMap</t>
+  </si>
+  <si>
+    <t>Program / Class =&gt; SyntaxLists</t>
+  </si>
+  <si>
+    <t>VersionedList&lt;All diagnostics&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1181,6 +1409,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1231,7 +1466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1270,6 +1505,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1554,10 +1800,10 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2264,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,7 +2813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2585,55 +2831,55 @@
     </row>
     <row r="2" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" t="s">
         <v>242</v>
-      </c>
-      <c r="D4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" t="s">
         <v>239</v>
-      </c>
-      <c r="D6" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="s">
         <v>236</v>
-      </c>
-      <c r="D8" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2643,15 +2889,15 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2659,65 +2905,65 @@
         <v>229</v>
       </c>
       <c r="C12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
+        <v>245</v>
+      </c>
+      <c r="D17" t="s">
         <v>246</v>
-      </c>
-      <c r="D17" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18" t="s">
         <v>250</v>
-      </c>
-      <c r="D18" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2727,163 +2973,163 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>252</v>
+      </c>
+      <c r="D22" t="s">
         <v>253</v>
-      </c>
-      <c r="D22" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
+        <v>259</v>
+      </c>
+      <c r="D26" t="s">
         <v>260</v>
-      </c>
-      <c r="D26" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>262</v>
+      </c>
+      <c r="D30" t="s">
         <v>263</v>
-      </c>
-      <c r="D30" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>265</v>
+      </c>
+      <c r="D32" t="s">
         <v>266</v>
-      </c>
-      <c r="D32" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>278</v>
+      </c>
+      <c r="D35" t="s">
         <v>279</v>
-      </c>
-      <c r="D35" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C38" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
+        <v>274</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C52" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C53" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2894,14 +3140,500 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="5" width="43" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="F4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="B5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="D5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="F5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="F6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="24" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="24" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="24" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="24" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>326</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C39" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>339</v>
+      </c>
+      <c r="C40" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>332</v>
+      </c>
+      <c r="C42" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="23" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>344</v>
+      </c>
+      <c r="D55" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>347</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>345</v>
+      </c>
+      <c r="C59" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="23" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="23" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>